<commit_message>
bug - CAPI_R122_C1	Rînd. 122 col.1	dec/DataSet/Data/CAPI_R122_C1
</commit_message>
<xml_diff>
--- a/2024/1 achiz pre re.xlsx
+++ b/2024/1 achiz pre re.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\work\1-achiz\2024\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC8E0F9B-638F-4788-A438-3CD21B22772D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0A9C6BB-0914-4E81-8916-5882A3889DBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4852" uniqueCount="2187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4852" uniqueCount="2188">
   <si>
     <t>title</t>
   </si>
@@ -6584,6 +6584,9 @@
   </si>
   <si>
     <t>dec/DataSet/Data/CAPI_R123_C2</t>
+  </si>
+  <si>
+    <t>dec/DataSet/Data/CAPI_R122_C1</t>
   </si>
 </sst>
 </file>
@@ -6984,8 +6987,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AE802"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A772" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A799" sqref="A799"/>
+    <sheetView tabSelected="1" topLeftCell="A787" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C802" sqref="C802"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -57114,7 +57117,7 @@
         <v>1132</v>
       </c>
       <c r="C801" s="4" t="s">
-        <v>2185</v>
+        <v>2187</v>
       </c>
       <c r="D801" s="4"/>
       <c r="E801" s="4"/>

</xml_diff>